<commit_message>
pin dimension! to integrate in the final common code
</commit_message>
<xml_diff>
--- a/output/PiN_JIAF_Somalia___SOM.xlsx
+++ b/output/PiN_JIAF_Somalia___SOM.xlsx
@@ -578,7 +578,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="35" customWidth="1" min="5" max="5"/>
+    <col width="23" customWidth="1" min="5" max="5"/>
     <col width="13" customWidth="1" min="6" max="6"/>
     <col width="18" customWidth="1" min="7" max="7"/>
     <col width="8" customWidth="1" min="8" max="8"/>
@@ -598,7 +598,7 @@
     <row r="1">
       <c r="E1" s="2" t="inlineStr">
         <is>
-          <t>PIN -- Host Community (5-17 y.o.)</t>
+          <t>PIN -- Host Community</t>
         </is>
       </c>
     </row>
@@ -2316,7 +2316,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="29" customWidth="1" min="5" max="5"/>
+    <col width="17" customWidth="1" min="5" max="5"/>
     <col width="13" customWidth="1" min="6" max="6"/>
     <col width="18" customWidth="1" min="7" max="7"/>
     <col width="7" customWidth="1" min="8" max="8"/>
@@ -2336,7 +2336,7 @@
     <row r="1">
       <c r="E1" s="2" t="inlineStr">
         <is>
-          <t>PIN -- New IDPs (5-17 y.o.)</t>
+          <t>PIN -- New IDPs</t>
         </is>
       </c>
     </row>
@@ -2915,7 +2915,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="36" customWidth="1" min="5" max="5"/>
+    <col width="24" customWidth="1" min="5" max="5"/>
     <col width="13" customWidth="1" min="6" max="6"/>
     <col width="18" customWidth="1" min="7" max="7"/>
     <col width="8" customWidth="1" min="8" max="8"/>
@@ -2935,7 +2935,7 @@
     <row r="1">
       <c r="E1" s="2" t="inlineStr">
         <is>
-          <t>PIN -- Protracted IDPs (5-17 y.o.)</t>
+          <t>PIN -- Protracted IDPs</t>
         </is>
       </c>
     </row>

</xml_diff>